<commit_message>
feat: add shipment type, shipment mode & mode of delivery to uploading data of rates to maintenance
</commit_message>
<xml_diff>
--- a/file-templates/published-rate-template.xlsx
+++ b/file-templates/published-rate-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wbms-cbl\file-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wbmsdiffs\wbms-toplist\file-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC783976-B9C6-4A50-8A50-D9A1374675AB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1B0688-80FC-4EB2-A8BC-E00C09D805C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" xr2:uid="{EC68E26C-5676-45B6-838C-33167DA3AE00}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC68E26C-5676-45B6-838C-33167DA3AE00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="49">
   <si>
     <t>TYPE</t>
   </si>
@@ -133,6 +133,51 @@
   </si>
   <si>
     <t>LBC</t>
+  </si>
+  <si>
+    <t>SHIPMENT TYPE</t>
+  </si>
+  <si>
+    <t>SHIPMENT MODE</t>
+  </si>
+  <si>
+    <t>MODE OF TRANSPORT</t>
+  </si>
+  <si>
+    <t>DOMESTIC</t>
+  </si>
+  <si>
+    <t>LCL</t>
+  </si>
+  <si>
+    <t>MOTORIZED COURIER</t>
+  </si>
+  <si>
+    <t>LAND FREIGHT</t>
+  </si>
+  <si>
+    <t>SEAFREIGHT DOMESTIC</t>
+  </si>
+  <si>
+    <t>AIRFREIGHT DOMESTIC</t>
+  </si>
+  <si>
+    <t>FCL</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL - IMPORT</t>
+  </si>
+  <si>
+    <t>SEAFREIGHT INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL - EXPORT</t>
+  </si>
+  <si>
+    <t>FTL</t>
+  </si>
+  <si>
+    <t>AIRFREGHT INTERNATIONAL</t>
   </si>
 </sst>
 </file>
@@ -140,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -210,19 +255,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -540,833 +585,1115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987498AE-F4FC-4FE8-9DB5-B961DF84AF8D}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>44.56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>64.239999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>52.56</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>71.239999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>62.56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>19</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>83.24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>19</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>62.56</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>83.24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>19</v>
       </c>
-      <c r="G10">
+      <c r="J10">
         <v>70.12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>19</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>72.36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>19</v>
       </c>
-      <c r="G12">
+      <c r="J12">
         <v>75.12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
+      <c r="H13" t="s">
         <v>22</v>
       </c>
-      <c r="F13" t="s">
+      <c r="I13" t="s">
         <v>19</v>
       </c>
-      <c r="G13">
+      <c r="J13">
         <v>77.36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>21</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>19</v>
       </c>
-      <c r="G14">
+      <c r="J14">
         <v>80.12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
         <v>22</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>19</v>
       </c>
-      <c r="G15">
+      <c r="J15">
         <v>82.36</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>21</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>19</v>
       </c>
-      <c r="G16">
+      <c r="J16">
         <v>80.12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
+      <c r="H17" t="s">
         <v>22</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I17" t="s">
         <v>19</v>
       </c>
-      <c r="G17">
+      <c r="J17">
         <v>82.36</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
         <v>17</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>24</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>1E-4</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>1</v>
       </c>
-      <c r="J18">
+      <c r="M18">
         <v>70.12</v>
       </c>
-      <c r="K18">
+      <c r="N18">
         <v>55.72</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
+      <c r="I19" t="s">
         <v>24</v>
       </c>
-      <c r="H19">
+      <c r="K19">
         <v>1E-4</v>
       </c>
-      <c r="I19">
+      <c r="L19">
         <v>1</v>
       </c>
-      <c r="J19">
+      <c r="M19">
         <v>75.12</v>
       </c>
-      <c r="K19">
+      <c r="N19">
         <v>55.72</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
         <v>26</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>24</v>
       </c>
-      <c r="H20">
+      <c r="K20">
         <v>1E-4</v>
       </c>
-      <c r="I20">
+      <c r="L20">
         <v>1</v>
       </c>
-      <c r="J20">
+      <c r="M20">
         <v>80.12</v>
       </c>
-      <c r="K20">
+      <c r="N20">
         <v>60.72</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
         <v>27</v>
       </c>
-      <c r="F21" t="s">
+      <c r="I21" t="s">
         <v>24</v>
       </c>
-      <c r="H21">
+      <c r="K21">
         <v>1E-4</v>
       </c>
-      <c r="I21">
+      <c r="L21">
         <v>1</v>
       </c>
-      <c r="J21">
+      <c r="M21">
         <v>80.12</v>
       </c>
-      <c r="K21">
+      <c r="N21">
         <v>60.72</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
         <v>29</v>
       </c>
-      <c r="E22" t="s">
+      <c r="H22" t="s">
         <v>31</v>
       </c>
-      <c r="F22" t="s">
+      <c r="I22" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="5">
+      <c r="J22" s="5">
         <v>379.5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
         <v>32</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
         <v>31</v>
       </c>
-      <c r="F23" t="s">
+      <c r="I23" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="3">
+      <c r="J23" s="3">
         <v>505.45</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
         <v>29</v>
       </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
         <v>30</v>
       </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>24</v>
       </c>
-      <c r="H24">
+      <c r="K24">
         <v>1E-4</v>
       </c>
-      <c r="I24">
+      <c r="L24">
         <v>0.5</v>
       </c>
-      <c r="J24">
+      <c r="M24">
         <v>379.5</v>
       </c>
-      <c r="K24">
+      <c r="N24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
         <v>29</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
         <v>30</v>
       </c>
-      <c r="F25" t="s">
+      <c r="I25" t="s">
         <v>24</v>
       </c>
-      <c r="H25">
+      <c r="K25">
         <v>0.50009999999999999</v>
       </c>
-      <c r="I25">
+      <c r="L25">
         <v>1</v>
       </c>
-      <c r="J25" s="3">
+      <c r="M25" s="3">
         <v>469.15</v>
       </c>
-      <c r="K25">
+      <c r="N25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
         <v>29</v>
       </c>
-      <c r="E26" t="s">
+      <c r="H26" t="s">
         <v>30</v>
       </c>
-      <c r="F26" t="s">
+      <c r="I26" t="s">
         <v>24</v>
       </c>
-      <c r="H26">
+      <c r="K26">
         <v>1.0001</v>
       </c>
-      <c r="I26">
+      <c r="L26">
         <v>1.5</v>
       </c>
-      <c r="J26" s="3">
+      <c r="M26" s="3">
         <v>560.45000000000005</v>
       </c>
-      <c r="K26">
+      <c r="N26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
         <v>29</v>
       </c>
-      <c r="E27" t="s">
+      <c r="H27" t="s">
         <v>30</v>
       </c>
-      <c r="F27" t="s">
+      <c r="I27" t="s">
         <v>24</v>
       </c>
-      <c r="H27">
+      <c r="K27">
         <v>1.5001</v>
       </c>
-      <c r="I27">
+      <c r="L27">
         <v>2</v>
       </c>
-      <c r="J27" s="3">
+      <c r="M27" s="3">
         <v>649</v>
       </c>
-      <c r="K27">
+      <c r="N27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
         <v>29</v>
       </c>
-      <c r="E28" t="s">
+      <c r="H28" t="s">
         <v>30</v>
       </c>
-      <c r="F28" t="s">
+      <c r="I28" t="s">
         <v>24</v>
       </c>
-      <c r="H28">
+      <c r="K28">
         <v>2.0001000000000002</v>
       </c>
-      <c r="I28">
+      <c r="L28">
         <v>2.5</v>
       </c>
-      <c r="J28" s="3">
+      <c r="M28" s="3">
         <v>738.1</v>
       </c>
-      <c r="K28">
+      <c r="N28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
         <v>23</v>
       </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
         <v>29</v>
       </c>
-      <c r="F29" t="s">
+      <c r="I29" t="s">
         <v>24</v>
       </c>
-      <c r="H29">
+      <c r="K29">
         <v>21</v>
       </c>
-      <c r="I29">
+      <c r="L29">
         <v>44</v>
       </c>
-      <c r="J29" s="4">
+      <c r="M29" s="4">
         <v>172.7</v>
       </c>
-      <c r="K29">
+      <c r="N29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
+      <c r="E30" t="s">
         <v>23</v>
       </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
         <v>29</v>
       </c>
-      <c r="F30" t="s">
+      <c r="I30" t="s">
         <v>24</v>
       </c>
-      <c r="H30">
+      <c r="K30">
         <v>45</v>
       </c>
-      <c r="I30">
+      <c r="L30">
         <v>70</v>
       </c>
-      <c r="J30" s="4">
+      <c r="M30" s="4">
         <v>169.95</v>
       </c>
-      <c r="K30">
+      <c r="N30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
+      <c r="E31" t="s">
         <v>23</v>
       </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
         <v>29</v>
       </c>
-      <c r="F31" t="s">
+      <c r="I31" t="s">
         <v>24</v>
       </c>
-      <c r="H31">
+      <c r="K31">
         <v>71</v>
       </c>
-      <c r="I31">
+      <c r="L31">
         <v>99</v>
       </c>
-      <c r="J31" s="4">
+      <c r="M31" s="4">
         <v>163.9</v>
       </c>
-      <c r="K31">
+      <c r="N31">
         <v>0</v>
       </c>
     </row>
@@ -1384,27 +1711,27 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>

</xml_diff>